<commit_message>
Refactor: updated suspended integration cases and fixed excel blank issue
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/CaseWorkerUserUpdateXlsxWithNoPassword.xlsx
+++ b/src/integrationTest/resources/CaseWorkerUserUpdateXlsxWithNoPassword.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93688AA-3C59-0048-90B5-CC031575974B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A676DB8D-BE90-A240-9F01-94F527289FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="1177">
   <si>
     <t>Region</t>
   </si>
@@ -4221,8 +4221,8 @@
   </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4341,11 +4341,11 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>6690mc</v>
+        <v>1348wv</v>
       </c>
       <c r="B2" s="1" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>1410jm</v>
+        <v>0546qw</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1176</v>
@@ -4377,9 +4377,7 @@
       <c r="K2" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>410</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>